<commit_message>
graph et truc que tu ecris dessus
</commit_message>
<xml_diff>
--- a/TP2/graphiques_seuils.xlsx
+++ b/TP2/graphiques_seuils.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leandre\Documents\Git\INF8775\TP2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antoine Gaulin\Documents\GitHub\INF8775\TP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2C558F86-3F34-4EDA-A7F9-67E0F3401A83}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E508A21-1250-4D79-B9E3-1F4BA649110F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="28800" windowHeight="16200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuille1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -46,11 +48,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="#,##0.00000"/>
-    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -371,7 +373,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -407,24 +409,24 @@
     </xf>
   </cellXfs>
   <cellStyles count="18">
-    <cellStyle name="Accent" xfId="7"/>
-    <cellStyle name="Accent 1" xfId="8"/>
-    <cellStyle name="Accent 2" xfId="9"/>
-    <cellStyle name="Accent 3" xfId="10"/>
-    <cellStyle name="Bad" xfId="4" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Error" xfId="11"/>
-    <cellStyle name="Footnote" xfId="12"/>
-    <cellStyle name="Good" xfId="3" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading (user)" xfId="13"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="14"/>
-    <cellStyle name="Neutral" xfId="5" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Accent 1" xfId="8" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent 3" xfId="10" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Error" xfId="11" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Footnote" xfId="12" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Heading (user)" xfId="13" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Hyperlink" xfId="14" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Insatisfaisant" xfId="4" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutre" xfId="5" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Note" xfId="6" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Status" xfId="15"/>
-    <cellStyle name="Text" xfId="16"/>
-    <cellStyle name="Warning" xfId="17"/>
+    <cellStyle name="Satisfaisant" xfId="3" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Status" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Text" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Titre 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titre 2" xfId="2" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Warning" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -442,7 +444,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -572,7 +574,7 @@
                       <a:latin typeface="Calibri"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="fr-FR"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -622,7 +624,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0" formatCode="#,##0.00000">
+                <c:pt idx="0" formatCode="#\ ##0.00000">
                   <c:v>2.9192399999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -656,6 +658,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D121-4855-BC54-338B171D54C2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -721,7 +728,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="#,##0.00000" sourceLinked="1"/>
+        <c:numFmt formatCode="#\ ##0.00000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -757,7 +764,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="407050032"/>
@@ -853,7 +860,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="407052656"/>
@@ -905,7 +912,7 @@
           <a:latin typeface="Calibri"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -919,7 +926,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -1049,7 +1056,7 @@
                       <a:latin typeface="Calibri"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="fr-FR"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1133,6 +1140,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-63E6-4A28-870D-94DEBAAF85DF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1234,7 +1246,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="407052000"/>
@@ -1330,7 +1342,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="407050688"/>
@@ -1382,7 +1394,7 @@
           <a:latin typeface="Calibri"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1396,7 +1408,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -1526,7 +1538,7 @@
                       <a:latin typeface="Calibri"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="fr-FR"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1610,6 +1622,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1762-4397-8251-BD7E414E2A8A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1711,7 +1728,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="407200848"/>
@@ -1807,7 +1824,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="407198880"/>
@@ -1859,7 +1876,7 @@
           <a:latin typeface="Calibri"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1873,7 +1890,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -1966,32 +1983,38 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuille1!$A$4:$A$11</c:f>
+              <c:f>Feuille1!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>10000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>30000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>100000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>300000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>1000000</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>3000000</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>6000000</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>8000000</c:v>
                 </c:pt>
               </c:numCache>
@@ -1999,38 +2022,49 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuille1!$B$15:$B$22</c:f>
+              <c:f>Feuille1!$B$13:$B$22</c:f>
               <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>0\.000000</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.3454944051395448E-3</c:v>
+                  <c:v>2.91924E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.455212518134125E-3</c:v>
+                  <c:v>2.7349633333333336E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4475952817051331E-3</c:v>
+                  <c:v>2.60516E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.4629020546118449E-3</c:v>
+                  <c:v>2.7613933333333336E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5123079555206696E-3</c:v>
+                  <c:v>2.79087E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5073726105194218E-3</c:v>
+                  <c:v>2.8437166666666668E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5404556623715808E-3</c:v>
+                  <c:v>2.9408500000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5642430466031869E-3</c:v>
+                  <c:v>2.9720633333333336E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.0351666666666665E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0736500000000003E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5D0A-4948-90EA-40F37460FB76}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2106,7 +2140,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+        <c:numFmt formatCode="0\.000000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -2142,7 +2176,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="407201176"/>
@@ -2237,7 +2271,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="407200192"/>
@@ -2289,7 +2323,7 @@
           <a:latin typeface="Calibri"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2303,7 +2337,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -2396,32 +2430,38 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuille1!$A$4:$A$11</c:f>
+              <c:f>Feuille1!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>10000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>30000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>100000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>300000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>1000000</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>3000000</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>6000000</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>8000000</c:v>
                 </c:pt>
               </c:numCache>
@@ -2429,38 +2469,49 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuille1!$C$15:$C$22</c:f>
+              <c:f>Feuille1!$C$13:$C$22</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>0\.0000</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3.356902662100289E-2</c:v>
+                  <c:v>3.4262899999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.4947915962275616E-2</c:v>
+                  <c:v>3.3873E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.4852869902497127E-2</c:v>
+                  <c:v>3.3476400000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4917860773463552E-2</c:v>
+                  <c:v>3.4840000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3667149888839433E-2</c:v>
+                  <c:v>3.4732699999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.3905696580515503E-2</c:v>
+                  <c:v>3.4785999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.4568477540480799E-2</c:v>
+                  <c:v>3.3527899999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.4048096372281046E-2</c:v>
+                  <c:v>3.3754333333333331E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.4407E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3886125000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0C4A-43D6-B3AC-21AF9275CA51}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2536,7 +2587,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:numFmt formatCode="0\.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -2572,7 +2623,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="407448672"/>
@@ -2667,7 +2718,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="407449984"/>
@@ -2719,7 +2770,7 @@
           <a:latin typeface="Calibri"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2733,7 +2784,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -2826,32 +2877,38 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuille1!$A$4:$A$11</c:f>
+              <c:f>Feuille1!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>10000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>30000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>100000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>300000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>1000000</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>3000000</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>6000000</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>8000000</c:v>
                 </c:pt>
               </c:numCache>
@@ -2859,38 +2916,49 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuille1!$D$15:$D$22</c:f>
+              <c:f>Feuille1!$D$13:$D$22</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>0\.0000</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.7757415968919018E-3</c:v>
+                  <c:v>3.3972999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8767294809448774E-3</c:v>
+                  <c:v>3.2518633333333334E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8657193050649751E-3</c:v>
+                  <c:v>3.08588E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.8659327902699717E-3</c:v>
+                  <c:v>3.2388133333333333E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.9614090807949592E-3</c:v>
+                  <c:v>3.2713999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.9598208420116064E-3</c:v>
+                  <c:v>3.3132399999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.9666712224339065E-3</c:v>
+                  <c:v>3.4713499999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0258159278503836E-3</c:v>
+                  <c:v>3.5136E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5499166666666665E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.6326875000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EB32-4DC5-98BC-910739635FEA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2966,7 +3034,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:numFmt formatCode="0\.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -3002,7 +3070,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="407451624"/>
@@ -3097,7 +3165,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="407450968"/>
@@ -3149,7 +3217,7 @@
           <a:latin typeface="Calibri"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3163,7 +3231,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -3286,40 +3354,46 @@
                       <a:latin typeface="Calibri"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="fr-FR"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuille1!$B$28:$B$35</c:f>
+              <c:f>Feuille1!$B$26:$B$35</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>11107.082559188651</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33741.19323200456</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>114024.97875611699</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>346386.08482319512</c:v>
+                  <c:v>30000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1170577.0359631393</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3555989.230556739</c:v>
+                  <c:v>300000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7168399.067039636</c:v>
+                  <c:v>1000000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9589262.6217990275</c:v>
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3330,7 +3404,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1112"/>
-                <c:pt idx="0" formatCode="#,##0.00000">
+                <c:pt idx="0" formatCode="#\ ##0.00000">
                   <c:v>2.9192399999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -3361,69 +3435,74 @@
                   <c:v>24589.200000000001</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.000000">
-                  <c:v>2.6981730565230643E-3</c:v>
+                  <c:v>2.91924E-3</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.000000">
-                  <c:v>2.4963893777797817E-3</c:v>
+                  <c:v>2.7349633333333336E-3</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.000000">
-                  <c:v>2.3454944051395448E-3</c:v>
+                  <c:v>2.60516E-3</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.000000">
-                  <c:v>2.455212518134125E-3</c:v>
+                  <c:v>2.7613933333333336E-3</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.000000">
-                  <c:v>2.4475952817051331E-3</c:v>
+                  <c:v>2.79087E-3</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.000000">
-                  <c:v>2.4629020546118449E-3</c:v>
+                  <c:v>2.8437166666666668E-3</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.000000">
-                  <c:v>2.5123079555206696E-3</c:v>
+                  <c:v>2.9408500000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.000000">
-                  <c:v>2.5073726105194218E-3</c:v>
+                  <c:v>2.9720633333333336E-3</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.000000">
-                  <c:v>2.5404556623715808E-3</c:v>
+                  <c:v>3.0351666666666665E-3</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.000000">
-                  <c:v>2.5642430466031869E-3</c:v>
+                  <c:v>3.0736500000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0">
-                  <c:v>1081.9320847276595</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0">
-                  <c:v>3286.7028168887655</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0">
-                  <c:v>11107.082559188651</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0">
-                  <c:v>33741.19323200456</c:v>
+                  <c:v>30000</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0">
-                  <c:v>114024.97875611699</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0">
-                  <c:v>346386.08482319512</c:v>
+                  <c:v>300000</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0">
-                  <c:v>1170577.0359631393</c:v>
+                  <c:v>1000000</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0">
-                  <c:v>3555989.230556739</c:v>
+                  <c:v>3000000</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0">
-                  <c:v>7168399.067039636</c:v>
+                  <c:v>6000000</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0">
-                  <c:v>9589262.6217990275</c:v>
+                  <c:v>8000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-376A-49A5-857A-3A3E50C2C089}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3535,7 +3614,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="407566656"/>
@@ -3641,7 +3720,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="407568296"/>
@@ -3693,7 +3772,7 @@
           <a:latin typeface="Calibri"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3707,7 +3786,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -3830,7 +3909,7 @@
                       <a:latin typeface="Calibri"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="fr-FR"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3842,28 +3921,28 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>9972.4071174155124</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29907.362748847081</c:v>
+                  <c:v>30000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>99655.20801347692</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>298867.10608374013</c:v>
+                  <c:v>300000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>995863.92405358935</c:v>
+                  <c:v>1000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2986607.2728968067</c:v>
+                  <c:v>3000000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5971972.5798814772</c:v>
+                  <c:v>6000000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7961942.9243831895</c:v>
+                  <c:v>8000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3902,6 +3981,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6AC7-4F00-A834-BF37CDA790CC}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4013,7 +4097,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="406596424"/>
@@ -4119,7 +4203,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="406594128"/>
@@ -4171,7 +4255,7 @@
           <a:latin typeface="Calibri"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4185,7 +4269,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -4308,7 +4392,7 @@
                       <a:latin typeface="Calibri"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="fr-FR"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4320,28 +4404,28 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>11117.317272815926</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33775.994803684436</c:v>
+                  <c:v>30000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>114156.33046188473</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>346823.2065227069</c:v>
+                  <c:v>300000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1172195.3655481304</c:v>
+                  <c:v>1000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3561296.6333584138</c:v>
+                  <c:v>3000000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7179595.7162133846</c:v>
+                  <c:v>6000000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9604516.8288363218</c:v>
+                  <c:v>8000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4380,6 +4464,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-23CB-4D21-B99A-57DAE7108FF8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4491,7 +4580,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="407567312"/>
@@ -4597,7 +4686,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="407566984"/>
@@ -4649,7 +4738,7 @@
           <a:latin typeface="Calibri"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4851,9 +4940,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
+      <xdr:colOff>857250</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>62904</xdr:rowOff>
+      <xdr:rowOff>177204</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5072908" cy="2766014"/>
     <xdr:graphicFrame macro="">
@@ -4881,10 +4970,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1552413</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>857088</xdr:colOff>
       <xdr:row>80</xdr:row>
-      <xdr:rowOff>161921</xdr:rowOff>
+      <xdr:rowOff>180971</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5096042" cy="2739377"/>
     <xdr:graphicFrame macro="">
@@ -4912,10 +5001,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>819153</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9528</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5124453" cy="2667003"/>
     <xdr:graphicFrame macro="">
@@ -4945,7 +5034,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5240,12 +5329,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1024" width="11" customWidth="1"/>
     <col min="1025" max="1025" width="9" customWidth="1"/>
@@ -5256,14 +5345,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="A1:D11"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R60" sqref="R60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="10.625" customWidth="1"/>
     <col min="2" max="2" width="14.75" customWidth="1"/>
@@ -5442,282 +5531,282 @@
     </row>
     <row r="13" spans="1:5">
       <c r="B13" s="4">
-        <f>B2/(A2^1.0114)</f>
-        <v>2.6981730565230643E-3</v>
+        <f>B2/(A2^1)</f>
+        <v>2.91924E-3</v>
       </c>
       <c r="C13" s="2">
-        <f>C2/(A2^0.9997)</f>
-        <v>3.4333977541006241E-2</v>
-      </c>
-      <c r="D13" s="2">
-        <f>D2/(A2^1.0115)</f>
-        <v>3.1378624283180108E-3</v>
+        <f>C2/(A2^1)</f>
+        <v>3.4262899999999999E-2</v>
+      </c>
+      <c r="D13" s="8">
+        <f>D2/(A2^1)</f>
+        <v>3.3972999999999998E-3</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="B14" s="4">
-        <f t="shared" ref="B14:B22" si="0">B3/(A3^1.0114)</f>
-        <v>2.4963893777797817E-3</v>
+        <f t="shared" ref="B14:B22" si="0">B3/(A3^1)</f>
+        <v>2.7349633333333336E-3</v>
       </c>
       <c r="C14" s="2">
-        <f t="shared" ref="C14:C22" si="1">C3/(A3^0.9997)</f>
-        <v>3.3954457694460247E-2</v>
-      </c>
-      <c r="D14" s="2">
-        <f t="shared" ref="D14:D22" si="2">D3/(A3^1.0115)</f>
-        <v>2.965824105513585E-3</v>
+        <f t="shared" ref="C14:C22" si="1">C3/(A3^1)</f>
+        <v>3.3873E-2</v>
+      </c>
+      <c r="D14" s="8">
+        <f t="shared" ref="D14:D22" si="2">D3/(A3^1)</f>
+        <v>3.2518633333333334E-3</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="B15" s="4">
         <f t="shared" si="0"/>
-        <v>2.3454944051395448E-3</v>
+        <v>2.60516E-3</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="1"/>
-        <v>3.356902662100289E-2</v>
-      </c>
-      <c r="D15" s="2">
+        <v>3.3476400000000003E-2</v>
+      </c>
+      <c r="D15" s="8">
         <f t="shared" si="2"/>
-        <v>2.7757415968919018E-3</v>
+        <v>3.08588E-3</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="B16" s="4">
         <f t="shared" si="0"/>
-        <v>2.455212518134125E-3</v>
+        <v>2.7613933333333336E-3</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="1"/>
-        <v>3.4947915962275616E-2</v>
-      </c>
-      <c r="D16" s="2">
+        <v>3.4840000000000003E-2</v>
+      </c>
+      <c r="D16" s="8">
         <f t="shared" si="2"/>
-        <v>2.8767294809448774E-3</v>
+        <v>3.2388133333333333E-3</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="4">
         <f t="shared" si="0"/>
-        <v>2.4475952817051331E-3</v>
+        <v>2.79087E-3</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="1"/>
-        <v>3.4852869902497127E-2</v>
-      </c>
-      <c r="D17" s="2">
+        <v>3.4732699999999998E-2</v>
+      </c>
+      <c r="D17" s="8">
         <f t="shared" si="2"/>
-        <v>2.8657193050649751E-3</v>
+        <v>3.2713999999999998E-3</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="4">
         <f t="shared" si="0"/>
-        <v>2.4629020546118449E-3</v>
+        <v>2.8437166666666668E-3</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="1"/>
-        <v>3.4917860773463552E-2</v>
-      </c>
-      <c r="D18" s="2">
+        <v>3.4785999999999997E-2</v>
+      </c>
+      <c r="D18" s="8">
         <f t="shared" si="2"/>
-        <v>2.8659327902699717E-3</v>
+        <v>3.3132399999999998E-3</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="4">
         <f t="shared" si="0"/>
-        <v>2.5123079555206696E-3</v>
+        <v>2.9408500000000001E-3</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" si="1"/>
-        <v>3.3667149888839433E-2</v>
-      </c>
-      <c r="D19" s="2">
+        <v>3.3527899999999999E-2</v>
+      </c>
+      <c r="D19" s="8">
         <f t="shared" si="2"/>
-        <v>2.9614090807949592E-3</v>
+        <v>3.4713499999999998E-3</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="4">
         <f t="shared" si="0"/>
-        <v>2.5073726105194218E-3</v>
+        <v>2.9720633333333336E-3</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" si="1"/>
-        <v>3.3905696580515503E-2</v>
-      </c>
-      <c r="D20" s="2">
+        <v>3.3754333333333331E-2</v>
+      </c>
+      <c r="D20" s="8">
         <f t="shared" si="2"/>
-        <v>2.9598208420116064E-3</v>
+        <v>3.5136E-3</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="4">
         <f t="shared" si="0"/>
-        <v>2.5404556623715808E-3</v>
+        <v>3.0351666666666665E-3</v>
       </c>
       <c r="C21" s="2">
         <f t="shared" si="1"/>
-        <v>3.4568477540480799E-2</v>
-      </c>
-      <c r="D21" s="2">
+        <v>3.4407E-2</v>
+      </c>
+      <c r="D21" s="8">
         <f t="shared" si="2"/>
-        <v>2.9666712224339065E-3</v>
+        <v>3.5499166666666665E-3</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="4">
         <f t="shared" si="0"/>
-        <v>2.5642430466031869E-3</v>
+        <v>3.0736500000000003E-3</v>
       </c>
       <c r="C22" s="2">
         <f t="shared" si="1"/>
-        <v>3.4048096372281046E-2</v>
-      </c>
-      <c r="D22" s="2">
+        <v>3.3886125000000003E-2</v>
+      </c>
+      <c r="D22" s="8">
         <f t="shared" si="2"/>
-        <v>3.0258159278503836E-3</v>
+        <v>3.6326875000000001E-3</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="3">
-        <f>(A2^1.0114)</f>
-        <v>1081.9320847276595</v>
+        <f>A2</f>
+        <v>1000</v>
       </c>
       <c r="C26" s="3">
-        <f>(A2^0.9997)</f>
-        <v>997.9298192025276</v>
+        <f>A2</f>
+        <v>1000</v>
       </c>
       <c r="D26" s="3">
-        <f>(A2^1.0115)</f>
-        <v>1082.6797151272995</v>
+        <f>A2</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="3">
-        <f t="shared" ref="B27:B35" si="3">(A3^1.0114)</f>
-        <v>3286.7028168887655</v>
+        <f t="shared" ref="B27:B35" si="3">A3</f>
+        <v>3000</v>
       </c>
       <c r="C27" s="3">
-        <f t="shared" ref="C27:C35" si="4">(A3^0.9997)</f>
-        <v>2992.8029160241717</v>
+        <f t="shared" ref="C27:C35" si="4">A3</f>
+        <v>3000</v>
       </c>
       <c r="D27" s="3">
-        <f t="shared" ref="D27:D35" si="5">(A3^1.0115)</f>
-        <v>3289.3353256735522</v>
+        <f t="shared" ref="D27:D35" si="5">A3</f>
+        <v>3000</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="3">
         <f t="shared" si="3"/>
-        <v>11107.082559188651</v>
+        <v>10000</v>
       </c>
       <c r="C28" s="3">
         <f t="shared" si="4"/>
-        <v>9972.4071174155124</v>
+        <v>10000</v>
       </c>
       <c r="D28" s="3">
         <f t="shared" si="5"/>
-        <v>11117.317272815926</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="3">
         <f t="shared" si="3"/>
-        <v>33741.19323200456</v>
+        <v>30000</v>
       </c>
       <c r="C29" s="3">
         <f t="shared" si="4"/>
-        <v>29907.362748847081</v>
+        <v>30000</v>
       </c>
       <c r="D29" s="3">
         <f t="shared" si="5"/>
-        <v>33775.994803684436</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" s="3">
         <f t="shared" si="3"/>
-        <v>114024.97875611699</v>
+        <v>100000</v>
       </c>
       <c r="C30" s="3">
         <f t="shared" si="4"/>
-        <v>99655.20801347692</v>
+        <v>100000</v>
       </c>
       <c r="D30" s="3">
         <f t="shared" si="5"/>
-        <v>114156.33046188473</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" s="3">
         <f t="shared" si="3"/>
-        <v>346386.08482319512</v>
+        <v>300000</v>
       </c>
       <c r="C31" s="3">
         <f t="shared" si="4"/>
-        <v>298867.10608374013</v>
+        <v>300000</v>
       </c>
       <c r="D31" s="3">
         <f t="shared" si="5"/>
-        <v>346823.2065227069</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="B32" s="3">
         <f t="shared" si="3"/>
-        <v>1170577.0359631393</v>
+        <v>1000000</v>
       </c>
       <c r="C32" s="3">
         <f t="shared" si="4"/>
-        <v>995863.92405358935</v>
+        <v>1000000</v>
       </c>
       <c r="D32" s="3">
         <f t="shared" si="5"/>
-        <v>1172195.3655481304</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="3">
         <f t="shared" si="3"/>
-        <v>3555989.230556739</v>
+        <v>3000000</v>
       </c>
       <c r="C33" s="3">
         <f t="shared" si="4"/>
-        <v>2986607.2728968067</v>
+        <v>3000000</v>
       </c>
       <c r="D33" s="3">
         <f t="shared" si="5"/>
-        <v>3561296.6333584138</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="34" spans="2:4">
       <c r="B34" s="3">
         <f t="shared" si="3"/>
-        <v>7168399.067039636</v>
+        <v>6000000</v>
       </c>
       <c r="C34" s="3">
         <f t="shared" si="4"/>
-        <v>5971972.5798814772</v>
+        <v>6000000</v>
       </c>
       <c r="D34" s="3">
         <f t="shared" si="5"/>
-        <v>7179595.7162133846</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="3">
         <f t="shared" si="3"/>
-        <v>9589262.6217990275</v>
+        <v>8000000</v>
       </c>
       <c r="C35" s="3">
         <f t="shared" si="4"/>
-        <v>7961942.9243831895</v>
+        <v>8000000</v>
       </c>
       <c r="D35" s="3">
         <f t="shared" si="5"/>
-        <v>9604516.8288363218</v>
+        <v>8000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>